<commit_message>
implemented actual time tracking, refactored variables in Main,arguments elsewhere
</commit_message>
<xml_diff>
--- a/ComputerTimeTracker/Data/Config.xlsx
+++ b/ComputerTimeTracker/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cito\Revature\Training\Team1EmptyString-P2\ComputerTimeTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18515EB6-EF8A-456C-8D7D-839D624289FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F193348B-36CF-409B-8AE3-0E52E877D68A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -171,6 +171,9 @@
   <si>
     <t>Time span representing how much time the time tracker should pause if it detects that all tracked apps are closed and the user chooses to continue tracking computer time.</t>
   </si>
+  <si>
+    <t>Notepad</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -242,6 +245,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -28515,7 +28519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -84252,10 +84256,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -84294,6 +84298,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="9">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
resolved some errors with getting event info, integrated ExceedTimeLimit workflow
</commit_message>
<xml_diff>
--- a/ComputerTimeTracker/Data/Config.xlsx
+++ b/ComputerTimeTracker/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cito\Revature\Training\Team1EmptyString-P2\ComputerTimeTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F193348B-36CF-409B-8AE3-0E52E877D68A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CF3211-3437-4D99-83DF-B6AB1F75AA1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -245,7 +245,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="46" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84259,13 +84259,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="8" customWidth="1"/>
     <col min="3" max="3" width="16.21875" customWidth="1"/>
     <col min="4" max="4" width="14.109375" customWidth="1"/>
   </cols>
@@ -84274,7 +84274,7 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -84289,7 +84289,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="5">
-        <v>6.9444444444444397E-3</v>
+        <v>1.1574074074074073E-4</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>0</v>
@@ -84302,7 +84302,7 @@
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="C3" t="b">

</xml_diff>

<commit_message>
implemented time tracking based on active window. this is interchangeable with time tracking based on user input event
</commit_message>
<xml_diff>
--- a/ComputerTimeTracker/Data/Config.xlsx
+++ b/ComputerTimeTracker/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cito\Revature\Training\Team1EmptyString-P2\ComputerTimeTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CF3211-3437-4D99-83DF-B6AB1F75AA1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF77F550-271E-438C-9AD6-0FF8948EAC51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -106,25 +106,16 @@
     <t>LogMessage_GetTransactionData</t>
   </si>
   <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
     <t>Static part of logging message. Calling Get Transaction Data.</t>
   </si>
   <si>
     <t>LogMessage_GetTransactionDataError</t>
   </si>
   <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
     <t>Static part of logging message. Error retrieving Transaction Data.</t>
   </si>
   <si>
     <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
   </si>
   <si>
     <t>Static part of logging message. Processed Transaction succesful.</t>
@@ -173,6 +164,15 @@
   </si>
   <si>
     <t>Notepad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing user input event at: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error getting transaction data at: </t>
+  </si>
+  <si>
+    <t>Successfully processed.</t>
   </si>
 </sst>
 </file>
@@ -28520,7 +28520,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="15" customHeight="1"/>
@@ -28694,10 +28694,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -28725,13 +28725,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -28759,13 +28759,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
@@ -28793,13 +28793,13 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
@@ -28827,13 +28827,13 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -28889,13 +28889,13 @@
     </row>
     <row r="12" spans="1:26" ht="28.2" customHeight="1">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" s="8">
         <v>5.7870370370370366E-5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -56232,7 +56232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -56247,10 +56247,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -84258,7 +84258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -84275,18 +84275,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5">
         <v>1.1574074074074073E-4</v>
@@ -84300,7 +84300,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8">
         <v>6.9444444444444441E-3</v>

</xml_diff>

<commit_message>
implemented website tracking, active window tracking
</commit_message>
<xml_diff>
--- a/ComputerTimeTracker/Data/Config.xlsx
+++ b/ComputerTimeTracker/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cito\Revature\Training\Team1EmptyString-P2\ComputerTimeTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF77F550-271E-438C-9AD6-0FF8948EAC51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521FF927-5DB3-4C7D-BEE8-F9D9917FC1D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Force Close</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>TimeDelayWhenAllAppsAreClosed</t>
   </si>
   <si>
@@ -173,6 +170,12 @@
   </si>
   <si>
     <t>Successfully processed.</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -28694,7 +28697,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
@@ -28728,7 +28731,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
@@ -28762,7 +28765,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -28889,13 +28892,13 @@
     </row>
     <row r="12" spans="1:26" ht="28.2" customHeight="1">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="8">
         <v>5.7870370370370366E-5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -56232,7 +56235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -84256,10 +84259,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -84286,7 +84289,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5">
         <v>1.1574074074074073E-4</v>
@@ -84300,7 +84303,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="8">
         <v>6.9444444444444441E-3</v>
@@ -84312,6 +84315,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implemented check if tracked websites are open
</commit_message>
<xml_diff>
--- a/ComputerTimeTracker/Data/Config.xlsx
+++ b/ComputerTimeTracker/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cito\Revature\Training\Team1EmptyString-P2\ComputerTimeTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521FF927-5DB3-4C7D-BEE8-F9D9917FC1D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9382F269-ADEE-4FF5-98CB-5B61A27EC0C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -175,7 +175,13 @@
     <t>Wikipedia</t>
   </si>
   <si>
-    <t>Chrome</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>App</t>
   </si>
 </sst>
 </file>
@@ -234,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -249,6 +255,8 @@
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="46" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84259,10 +84267,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -84273,7 +84281,7 @@
     <col min="4" max="4" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -84286,8 +84294,11 @@
       <c r="D1" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -84300,8 +84311,11 @@
       <c r="D2" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -84314,20 +84328,12 @@
       <c r="D3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>38</v>
+      <c r="E3" s="11" t="s">
+        <v>40</v>
       </c>
-      <c r="B4" s="8">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="E4" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
refined workflow logic, tracked apps are now configured from storage bucket
</commit_message>
<xml_diff>
--- a/ComputerTimeTracker/Data/Config.xlsx
+++ b/ComputerTimeTracker/Data/Config.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cito\Revature\Training\Team1EmptyString-P2\ComputerTimeTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442F12EC-C5CA-409E-A801-A5D0A14E3F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702AEC56-3E50-4B67-84F4-69747ECDE0EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
-    <sheet name="TrackedApps" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -145,22 +144,10 @@
     <t>Description (Assets will always overwrite other config)</t>
   </si>
   <si>
-    <t>Time Limit</t>
-  </si>
-  <si>
-    <t>Notification</t>
-  </si>
-  <si>
-    <t>Force Close</t>
-  </si>
-  <si>
     <t>TimeDelayWhenAllAppsAreClosed</t>
   </si>
   <si>
     <t>Time span representing how much time the time tracker should pause if it detects that all tracked apps are closed and the user chooses to continue tracking computer time.</t>
-  </si>
-  <si>
-    <t>Notepad</t>
   </si>
   <si>
     <t xml:space="preserve">Processing user input event at: </t>
@@ -172,26 +159,32 @@
     <t>Successfully processed.</t>
   </si>
   <si>
-    <t>Wikipedia</t>
+    <t>TimeoutForHTML_ElementMS</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>TrackedAppsFileName</t>
   </si>
   <si>
-    <t>Website</t>
+    <t>TrackedApps.xlsx</t>
   </si>
   <si>
-    <t>App</t>
+    <t>Name of file in Orchestrator storage that contains settings for which apps to track.</t>
   </si>
   <si>
-    <t>TimeoutForHTML_ElementMS</t>
+    <t>TrackedAppsStorageBucket</t>
+  </si>
+  <si>
+    <t>TrackedAppsSettings</t>
+  </si>
+  <si>
+    <t>Name of storage bucket in Orchestrator which contains the TrackedApps file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -211,13 +204,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -243,23 +229,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="46" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,7 +557,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="15" customHeight="1"/>
@@ -747,9 +727,15 @@
       <c r="Z5"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
@@ -775,9 +761,15 @@
       <c r="Z6"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
@@ -28533,7 +28525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -28708,7 +28700,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
@@ -28742,7 +28734,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
@@ -28776,7 +28768,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -28903,13 +28895,13 @@
     </row>
     <row r="12" spans="1:26" ht="28.2" customHeight="1">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="5">
         <v>5.7870370370370366E-5</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>32</v>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -28937,7 +28929,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -56250,7 +56242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -84270,80 +84262,4 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1.1574074074074073E-4</v>
-      </c>
-      <c r="C2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="8">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="E4" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>